<commit_message>
1) Tournment. 2) score, rank, brief in STAT
</commit_message>
<xml_diff>
--- a/IPL Error Codes.xlsx
+++ b/IPL Error Codes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="4"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="PLAYER" sheetId="5" r:id="rId6"/>
     <sheet name="AUCTION" sheetId="6" r:id="rId7"/>
     <sheet name="STAT" sheetId="8" r:id="rId8"/>
+    <sheet name="TOURNAMENT" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>User does not belong to group 1</t>
   </si>
@@ -115,6 +116,15 @@
   </si>
   <si>
     <t>Unable to connect to CricAPI</t>
+  </si>
+  <si>
+    <t>720 series</t>
+  </si>
+  <si>
+    <t>640 series</t>
+  </si>
+  <si>
+    <t>Invalid tournament name</t>
   </si>
 </sst>
 </file>
@@ -683,10 +693,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,6 +713,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -712,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -871,7 +886,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -891,6 +906,47 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>741</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added user name, player name in stat output
</commit_message>
<xml_diff>
--- a/IPL Error Codes.xlsx
+++ b/IPL Error Codes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>User does not belong to group 1</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Invalid tournament name</t>
+  </si>
+  <si>
+    <t>Invalid User id</t>
+  </si>
+  <si>
+    <t>Invalid gounp number</t>
   </si>
 </sst>
 </file>
@@ -888,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,6 +912,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>721</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>722</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
@@ -920,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
playerCount in /balance & max player purchase chk
</commit_message>
<xml_diff>
--- a/IPL Error Codes.xlsx
+++ b/IPL Error Codes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>User does not belong to group 1</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Max Wicket already assigned</t>
+  </si>
+  <si>
+    <t>Max player purchase count reached. Cannot buy additional player.</t>
   </si>
 </sst>
 </file>
@@ -810,16 +813,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -894,6 +897,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>709</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -903,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>